<commit_message>
Final fixes to escape tests
</commit_message>
<xml_diff>
--- a/data/escape.xlsx
+++ b/data/escape.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee85442dac9ca7a7/Documents/Julia/XLSX/XLSX.jl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{FFD7FC4C-166E-4686-9EBB-879BC88BA5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E21AB69D-DEF9-458C-AFB2-B8B108AD8CFA}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
-    <sheet name="&amp;; &amp;amp; &amp;quot; &amp;lt; &amp;gt; &amp;apos; I❤Julia&quot;&lt;'&amp;O-O&amp;'&gt;&quot;&lt;&amp;&gt;" sheetId="1" r:id="rId1"/>
+    <sheet name="&amp; &amp; &quot; &gt; &lt; " sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
-  <si>
-    <t>&amp;; &amp;amp; &amp;quot; &amp;lt; &amp;gt; &amp;apos; </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>I❤Julia</t>
   </si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>45' '; ''</t>
+  </si>
+  <si>
+    <t>&amp;&amp;apos; &amp;amp; &amp;quot; &amp;lt; &amp;gt; &amp;apos;</t>
   </si>
 </sst>
 </file>
@@ -151,10 +151,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -192,7 +196,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -298,7 +302,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -440,7 +444,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -452,90 +456,90 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove dependency on ZipFiles.jl and EzXML.jl (#280)
* Remove remaining dependency on ZipFile.jl

* Remove overlooked use of ZipFile

* No need to close zip io any longer

* No need to close zip io any longer

* Now also removed dependency on EzXML.jl except for calls to the
 overloaded findall() and findfirst() functions and a single call
 to EzXMLunlnk().

* Replace EzXML.findall() with a new find_all_nodes()
function that uses the XML.jl API.

* Replaced EzXML.findfirst() with find_all_nodes()[begin]

* Further changes to unlink rows in write.jl

* Yesterday's changes

* Finally got SheetRowStreamIterator to work!

* Further changes bug fixing failed tests

* Force recompile?

* Now passing all tests except `escape`

* Clean up remaining open and close actions

* Final fixes to escape tests

* Remove unnecesaary data files

* Tidy-up

* Don't pretty print

* Remove last pretty printing example

* Simplify regex that undoes pretty printing
</commit_message>
<xml_diff>
--- a/data/escape.xlsx
+++ b/data/escape.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/felipenoris/tmp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/ee85442dac9ca7a7/Documents/Julia/XLSX/XLSX.jl/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C353BCB8-5EC8-0143-BDD3-A1B661DAACD7}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="8_{FFD7FC4C-166E-4686-9EBB-879BC88BA5C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E21AB69D-DEF9-458C-AFB2-B8B108AD8CFA}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{52D9C27D-0EF6-DD41-9728-0267E68F7539}"/>
   </bookViews>
   <sheets>
-    <sheet name="&amp;; &amp;amp; &amp;quot; &amp;lt; &amp;gt; &amp;apos; I❤Julia&quot;&lt;'&amp;O-O&amp;'&gt;&quot;&lt;&amp;&gt;" sheetId="1" r:id="rId1"/>
+    <sheet name="&amp; &amp; &quot; &gt; &lt; " sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,10 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="24">
-  <si>
-    <t>&amp;; &amp;amp; &amp;quot; &amp;lt; &amp;gt; &amp;apos; </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>I❤Julia</t>
   </si>
@@ -97,6 +94,9 @@
   </si>
   <si>
     <t>45' '; ''</t>
+  </si>
+  <si>
+    <t>&amp;&amp;apos; &amp;amp; &amp;quot; &amp;lt; &amp;gt; &amp;apos;</t>
   </si>
 </sst>
 </file>
@@ -151,10 +151,14 @@
 </styleSheet>
 </file>
 
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -192,7 +196,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -298,7 +302,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -440,7 +444,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -452,90 +456,90 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
+        <v>6</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>7</v>
       </c>
+      <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>9</v>
+      </c>
+      <c r="D3" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="3" spans="1:4">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" t="s">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>11</v>
       </c>
+      <c r="B4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="4" spans="1:4">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>15</v>
       </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
-        <v>16</v>
-      </c>
-      <c r="B5" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
+      <c r="B6" t="s">
         <v>20</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
         <v>21</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>22</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>